<commit_message>
Adds inventories of Wolff et al. 2020
</commit_message>
<xml_diff>
--- a/dev/Assumptions and data.xlsx
+++ b/dev/Assumptions and data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Documents\GitHub\carculator_truck\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAA09F7-5ED6-4BA4-A010-E4129CF97F34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C533E3B5-2453-4232-BA35-41E56A18CD3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{F660A75E-F0EB-488E-A727-CFDC76EA02DE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="5" xr2:uid="{F660A75E-F0EB-488E-A727-CFDC76EA02DE}"/>
   </bookViews>
   <sheets>
     <sheet name="ICEV engines" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Loading factors" sheetId="5" r:id="rId4"/>
     <sheet name="battery sizing" sheetId="6" r:id="rId5"/>
     <sheet name="weight composition" sheetId="7" r:id="rId6"/>
+    <sheet name="weight composition of MAN TGX" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="159">
   <si>
     <t>kW</t>
   </si>
@@ -346,9 +347,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Cabin</t>
   </si>
   <si>
@@ -455,20 +453,84 @@
   </si>
   <si>
     <t>Toyota Prius</t>
+  </si>
+  <si>
+    <t>Total, incl. Trailer</t>
+  </si>
+  <si>
+    <t>Trailer</t>
+  </si>
+  <si>
+    <t>Tractor</t>
+  </si>
+  <si>
+    <t>Trailer, % weight</t>
+  </si>
+  <si>
+    <t>of which, Frame</t>
+  </si>
+  <si>
+    <t>of which, Suspension</t>
+  </si>
+  <si>
+    <t>of which, Wheels and tires</t>
+  </si>
+  <si>
+    <t>of which, Brakes</t>
+  </si>
+  <si>
+    <t>of which, Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E.G., MAN TGX </t>
+  </si>
+  <si>
+    <t>Scaling Factor</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Mass [kg]</t>
+  </si>
+  <si>
+    <t>Engine &amp; Exhaust system*</t>
+  </si>
+  <si>
+    <t>Cab</t>
+  </si>
+  <si>
+    <t>Tires &amp; Wheels</t>
+  </si>
+  <si>
+    <t>Diesel/Adbluetank</t>
+  </si>
+  <si>
+    <t>Gearbox</t>
+  </si>
+  <si>
+    <t>Retarder</t>
+  </si>
+  <si>
+    <t>Total [kg]</t>
+  </si>
+  <si>
+    <t>Wolff et al. 2020, Sustainability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,8 +578,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -542,8 +620,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -575,6 +671,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -584,7 +704,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -649,6 +769,25 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2689,55 +2828,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.5</c:v>
+                  <c:v>3500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5</c:v>
+                  <c:v>7500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>12000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>18000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>26000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'weight composition'!$F$24:$L$24</c:f>
+              <c:f>'weight composition'!$F$31:$L$31</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>150.79166666666669</c:v>
+                  <c:v>82.541666666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>323.125</c:v>
+                  <c:v>176.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>517</c:v>
+                  <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>775.5</c:v>
+                  <c:v>424.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1120.1666666666665</c:v>
+                  <c:v>613.16666666666663</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>998</c:v>
+                  <c:v>558</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1497</c:v>
+                  <c:v>837</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5888,15 +6027,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>511175</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>58737</xdr:rowOff>
+      <xdr:colOff>454025</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>122237</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>530225</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>93662</xdr:rowOff>
+      <xdr:colOff>473075</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6223,7 +6362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A40BBB6-5CB6-4687-8C18-59866161D37E}">
   <dimension ref="A2:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
@@ -6244,7 +6383,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -6282,28 +6421,28 @@
         <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -6426,7 +6565,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -6434,16 +6573,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -6504,19 +6643,19 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" t="s">
         <v>137</v>
-      </c>
-      <c r="C6" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -9364,15 +9503,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FC8F20-42EB-4BE3-A713-D92C184011E3}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="10" width="18.6328125" customWidth="1"/>
     <col min="11" max="12" width="12.6328125" bestFit="1" customWidth="1"/>
@@ -9380,64 +9519,64 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" t="s">
         <v>118</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" t="s">
         <v>119</v>
       </c>
-      <c r="H4" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>120</v>
-      </c>
-      <c r="J4" t="s">
-        <v>121</v>
       </c>
       <c r="K4" s="34" t="s">
         <v>97</v>
       </c>
       <c r="L4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F5">
-        <v>3.5</v>
+        <v>3500</v>
       </c>
       <c r="G5">
-        <v>7.5</v>
+        <v>7500</v>
       </c>
       <c r="H5" s="34">
-        <v>12</v>
+        <v>12000</v>
       </c>
       <c r="I5">
-        <v>18</v>
+        <v>18000</v>
       </c>
       <c r="J5">
-        <v>26</v>
+        <v>26000</v>
       </c>
       <c r="K5" s="34">
-        <v>40</v>
+        <v>40000</v>
       </c>
       <c r="L5">
-        <v>60</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -9445,7 +9584,7 @@
         <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F6" s="8">
         <f>H6*$F$5/$H$5</f>
@@ -9476,7 +9615,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" s="8">
         <f t="shared" ref="F7:F18" si="0">H7*$F$5/$H$5</f>
@@ -9507,7 +9646,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" s="8">
         <f t="shared" si="0"/>
@@ -9538,7 +9677,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" s="8">
         <f t="shared" si="0"/>
@@ -9569,7 +9708,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" s="8">
         <f t="shared" si="0"/>
@@ -9634,7 +9773,7 @@
         <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F12" s="8">
         <f t="shared" si="0"/>
@@ -9665,7 +9804,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F13" s="8">
         <f t="shared" si="0"/>
@@ -9696,7 +9835,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F14" s="8">
         <f t="shared" si="0"/>
@@ -9727,7 +9866,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="E15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" si="0"/>
@@ -9758,10 +9897,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" si="0"/>
@@ -9792,7 +9931,7 @@
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.35">
       <c r="E17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="0"/>
@@ -9827,297 +9966,738 @@
       </c>
       <c r="F18" s="8">
         <f t="shared" si="0"/>
-        <v>583.33333333333337</v>
+        <v>659.16666666666663</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" si="1"/>
-        <v>1250</v>
+        <v>1412.5</v>
       </c>
       <c r="H18" s="35">
-        <v>2000</v>
+        <v>2260</v>
       </c>
       <c r="I18" s="8">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>3390</v>
       </c>
       <c r="J18" s="8">
         <f t="shared" si="3"/>
-        <v>4333.333333333333</v>
+        <v>4896.666666666667</v>
       </c>
       <c r="K18" s="35">
-        <v>2100</v>
+        <v>2700</v>
       </c>
       <c r="L18" s="8">
         <f t="shared" si="4"/>
-        <v>3150</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="F19" s="8">
         <f t="shared" ref="F19:L19" si="5">SUM(F6:F18)</f>
-        <v>1732.5</v>
+        <v>1808.3333333333335</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" si="5"/>
-        <v>3712.5</v>
+        <v>3875</v>
       </c>
       <c r="H19" s="35">
         <f t="shared" si="5"/>
-        <v>5940</v>
+        <v>6200</v>
       </c>
       <c r="I19" s="8">
         <f t="shared" si="5"/>
-        <v>8910</v>
+        <v>9300</v>
       </c>
       <c r="J19" s="8">
         <f t="shared" si="5"/>
-        <v>12870</v>
+        <v>13433.333333333332</v>
       </c>
       <c r="K19" s="35">
         <f t="shared" si="5"/>
-        <v>13941</v>
+        <v>14541</v>
       </c>
       <c r="L19" s="8">
         <f t="shared" si="5"/>
-        <v>20911.5</v>
+        <v>21811.5</v>
       </c>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="8">
+        <f>F5-F19</f>
+        <v>1691.6666666666665</v>
+      </c>
+      <c r="G20" s="8">
+        <f>G5-G19</f>
+        <v>3625</v>
+      </c>
+      <c r="H20" s="8">
+        <f>H5-H19</f>
+        <v>5800</v>
+      </c>
+      <c r="I20" s="8">
+        <f>I5-I19</f>
+        <v>8700</v>
+      </c>
+      <c r="J20" s="8">
+        <f>J5-J19</f>
+        <v>12566.666666666668</v>
+      </c>
+      <c r="K20" s="8">
+        <f>K5-K19</f>
+        <v>25459</v>
+      </c>
+      <c r="L20" s="8">
+        <f>L5-L19</f>
+        <v>38188.5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="8">
+        <f>F19-F28</f>
+        <v>495.83333333333348</v>
+      </c>
+      <c r="G21" s="8">
+        <f>G19-G28</f>
+        <v>1062.5</v>
+      </c>
+      <c r="H21" s="8">
+        <f>H19-H28</f>
+        <v>1700</v>
+      </c>
+      <c r="I21" s="8">
+        <f t="shared" ref="I21:J21" si="6">I19-I28</f>
+        <v>2550</v>
+      </c>
+      <c r="J21" s="8">
+        <f t="shared" si="6"/>
+        <v>3683.3333333333321</v>
+      </c>
+      <c r="K21" s="35">
+        <f>K19-7050</f>
+        <v>7491</v>
+      </c>
+      <c r="L21" s="39">
+        <f>L19-7050</f>
+        <v>14761.5</v>
+      </c>
+    </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="38">
+        <f t="shared" ref="F22:K22" si="7">F21/F19</f>
+        <v>0.27419354838709681</v>
+      </c>
+      <c r="G22" s="38">
+        <f t="shared" si="7"/>
+        <v>0.27419354838709675</v>
+      </c>
+      <c r="H22" s="38">
+        <f t="shared" si="7"/>
+        <v>0.27419354838709675</v>
+      </c>
+      <c r="I22" s="38">
+        <f t="shared" si="7"/>
+        <v>0.27419354838709675</v>
+      </c>
+      <c r="J22" s="38">
+        <f t="shared" si="7"/>
+        <v>0.2741935483870967</v>
+      </c>
+      <c r="K22" s="38">
+        <f t="shared" si="7"/>
+        <v>0.51516401898081288</v>
+      </c>
+      <c r="L22" s="38">
+        <f>L21/L19</f>
+        <v>0.67677601265387521</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D23" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" s="41">
+        <f t="shared" ref="F23:H27" si="8">$K23*F$21/$K$21</f>
+        <v>171.10254527655414</v>
+      </c>
+      <c r="G23" s="41">
+        <f t="shared" si="8"/>
+        <v>366.64831130690163</v>
+      </c>
+      <c r="H23" s="41">
+        <f t="shared" si="8"/>
+        <v>586.63729809104257</v>
+      </c>
+      <c r="I23" s="41">
+        <f>$K23*I$21/$K$21</f>
+        <v>879.95594713656385</v>
+      </c>
+      <c r="J23" s="41">
+        <f>$K23*J$21/$K$21</f>
+        <v>1271.0474791972586</v>
+      </c>
+      <c r="K23" s="41">
+        <f>K12-854</f>
+        <v>2585</v>
+      </c>
+      <c r="L23" s="41">
+        <f>K23*$L$21/$K$21</f>
+        <v>5093.9096916299559</v>
+      </c>
+    </row>
+    <row r="24" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D24" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="41">
+        <f t="shared" si="8"/>
+        <v>69.89720998531574</v>
+      </c>
+      <c r="G24" s="41">
+        <f t="shared" si="8"/>
+        <v>149.77973568281939</v>
+      </c>
+      <c r="H24" s="41">
+        <f t="shared" si="8"/>
+        <v>239.647577092511</v>
+      </c>
+      <c r="I24" s="41">
+        <f t="shared" ref="I24:I27" si="9">$K24*I$21/$K$21</f>
+        <v>359.47136563876654</v>
+      </c>
+      <c r="J24" s="41">
+        <f t="shared" ref="J24:J27" si="10">$K24*J$21/$K$21</f>
+        <v>519.23641703377371</v>
+      </c>
+      <c r="K24" s="41">
+        <f>K13-1600</f>
+        <v>1056</v>
+      </c>
+      <c r="L24" s="41">
+        <f t="shared" ref="L24:L27" si="11">K24*$L$21/$K$21</f>
+        <v>2080.9162995594716</v>
+      </c>
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D25" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="41">
+        <f t="shared" si="8"/>
+        <v>50.503381835980967</v>
+      </c>
+      <c r="G25" s="41">
+        <f t="shared" si="8"/>
+        <v>108.22153250567348</v>
+      </c>
+      <c r="H25" s="41">
+        <f t="shared" si="8"/>
+        <v>173.15445200907757</v>
+      </c>
+      <c r="I25" s="41">
+        <f t="shared" si="9"/>
+        <v>259.73167801361632</v>
+      </c>
+      <c r="J25" s="41">
+        <f t="shared" si="10"/>
+        <v>375.16797935300127</v>
+      </c>
+      <c r="K25" s="41">
+        <f>K15-659</f>
+        <v>763</v>
+      </c>
+      <c r="L25" s="41">
+        <f t="shared" si="11"/>
+        <v>1503.5408490188227</v>
+      </c>
+    </row>
+    <row r="26" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D26" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" s="41">
+        <f t="shared" si="8"/>
+        <v>26.733603832840483</v>
+      </c>
+      <c r="G26" s="41">
+        <f t="shared" si="8"/>
+        <v>57.286293927515295</v>
+      </c>
+      <c r="H26" s="41">
+        <f t="shared" si="8"/>
+        <v>91.658070284024475</v>
+      </c>
+      <c r="I26" s="41">
+        <f t="shared" si="9"/>
+        <v>137.48710542603672</v>
+      </c>
+      <c r="J26" s="41">
+        <f t="shared" si="10"/>
+        <v>198.59248561538632</v>
+      </c>
+      <c r="K26" s="41">
+        <f>K14*K22</f>
+        <v>403.88859088095728</v>
+      </c>
+      <c r="L26" s="41">
+        <f t="shared" si="11"/>
+        <v>795.88859088095717</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D27" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="41">
+        <f t="shared" si="8"/>
+        <v>178.71445734881866</v>
+      </c>
+      <c r="G27" s="41">
+        <f t="shared" si="8"/>
+        <v>382.95955146175413</v>
+      </c>
+      <c r="H27" s="41">
+        <f t="shared" si="8"/>
+        <v>612.73528233880654</v>
+      </c>
+      <c r="I27" s="41">
+        <f t="shared" si="9"/>
+        <v>919.10292350820987</v>
+      </c>
+      <c r="J27" s="41">
+        <f t="shared" si="10"/>
+        <v>1327.5931117340804</v>
+      </c>
+      <c r="K27" s="41">
+        <f>K18</f>
+        <v>2700</v>
+      </c>
+      <c r="L27" s="41">
+        <f t="shared" si="11"/>
+        <v>5320.5246295554662</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>140</v>
+      </c>
+      <c r="F28" s="8">
+        <f>H28*$F$5/$H$5</f>
+        <v>1312.5</v>
+      </c>
+      <c r="G28" s="8">
+        <f>H28*$G$5/$H$5</f>
+        <v>2812.5</v>
+      </c>
+      <c r="H28" s="34">
+        <v>4500</v>
+      </c>
+      <c r="I28" s="8">
+        <f>H28*$I$5/$H$5</f>
+        <v>6750</v>
+      </c>
+      <c r="J28" s="8">
+        <f>H28*$J$5/$H$5</f>
+        <v>9750</v>
+      </c>
+      <c r="K28" s="35">
+        <f>K19-K21</f>
+        <v>7050</v>
+      </c>
+      <c r="L28" s="39">
+        <f>L19-L21</f>
+        <v>7050</v>
+      </c>
+    </row>
+    <row r="30" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
         <v>123</v>
       </c>
-      <c r="F20" s="8">
-        <f t="shared" ref="F20:L20" si="6">(F5*1000)-F19</f>
-        <v>1767.5</v>
-      </c>
-      <c r="G20" s="8">
-        <f t="shared" si="6"/>
-        <v>3787.5</v>
-      </c>
-      <c r="H20" s="8">
-        <f t="shared" si="6"/>
-        <v>6060</v>
-      </c>
-      <c r="I20" s="8">
-        <f t="shared" si="6"/>
-        <v>9090</v>
-      </c>
-      <c r="J20" s="8">
-        <f t="shared" si="6"/>
-        <v>13130</v>
-      </c>
-      <c r="K20" s="8">
-        <f t="shared" si="6"/>
-        <v>26059</v>
-      </c>
-      <c r="L20" s="8">
-        <f t="shared" si="6"/>
-        <v>39088.5</v>
-      </c>
-    </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D23" t="s">
+      <c r="F30" s="8">
+        <f>SUM(F11:F18)</f>
+        <v>1506.4583333333333</v>
+      </c>
+      <c r="G30" s="8">
+        <f t="shared" ref="G30:L30" si="12">SUM(G11:G18)</f>
+        <v>3228.125</v>
+      </c>
+      <c r="H30" s="8">
+        <f t="shared" si="12"/>
+        <v>5165</v>
+      </c>
+      <c r="I30" s="8">
+        <f t="shared" si="12"/>
+        <v>7747.5</v>
+      </c>
+      <c r="J30" s="8">
+        <f t="shared" si="12"/>
+        <v>11190.833333333334</v>
+      </c>
+      <c r="K30" s="8">
+        <f t="shared" si="12"/>
+        <v>12419</v>
+      </c>
+      <c r="L30" s="8">
+        <f t="shared" si="12"/>
+        <v>18628.5</v>
+      </c>
+    </row>
+    <row r="31" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="8">
-        <f>SUM(F11:F18)</f>
-        <v>1430.625</v>
-      </c>
-      <c r="G23" s="8">
-        <f t="shared" ref="G23:L23" si="7">SUM(G11:G18)</f>
-        <v>3065.625</v>
-      </c>
-      <c r="H23" s="8">
-        <f t="shared" si="7"/>
-        <v>4905</v>
-      </c>
-      <c r="I23" s="8">
-        <f t="shared" si="7"/>
-        <v>7357.5</v>
-      </c>
-      <c r="J23" s="8">
-        <f t="shared" si="7"/>
-        <v>10627.5</v>
-      </c>
-      <c r="K23" s="8">
-        <f t="shared" si="7"/>
-        <v>11819</v>
-      </c>
-      <c r="L23" s="8">
-        <f t="shared" si="7"/>
-        <v>17728.5</v>
-      </c>
-    </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D24" t="s">
+      <c r="F31" s="8">
+        <f>SUM(F10)</f>
+        <v>82.541666666666671</v>
+      </c>
+      <c r="G31" s="8">
+        <f t="shared" ref="G31:L31" si="13">SUM(G10)</f>
+        <v>176.875</v>
+      </c>
+      <c r="H31" s="8">
+        <f t="shared" si="13"/>
+        <v>283</v>
+      </c>
+      <c r="I31" s="8">
+        <f t="shared" si="13"/>
+        <v>424.5</v>
+      </c>
+      <c r="J31" s="8">
+        <f t="shared" si="13"/>
+        <v>613.16666666666663</v>
+      </c>
+      <c r="K31" s="8">
+        <f t="shared" si="13"/>
+        <v>558</v>
+      </c>
+      <c r="L31" s="8">
+        <f t="shared" si="13"/>
+        <v>837</v>
+      </c>
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
         <v>125</v>
       </c>
-      <c r="F24" s="8">
-        <f>SUM(F7:F10)</f>
-        <v>150.79166666666669</v>
-      </c>
-      <c r="G24" s="8">
-        <f t="shared" ref="G24:L24" si="8">SUM(G7:G10)</f>
-        <v>323.125</v>
-      </c>
-      <c r="H24" s="8">
-        <f t="shared" si="8"/>
-        <v>517</v>
-      </c>
-      <c r="I24" s="8">
-        <f t="shared" si="8"/>
-        <v>775.5</v>
-      </c>
-      <c r="J24" s="8">
-        <f t="shared" si="8"/>
-        <v>1120.1666666666665</v>
-      </c>
-      <c r="K24" s="8">
-        <f t="shared" si="8"/>
-        <v>998</v>
-      </c>
-      <c r="L24" s="8">
-        <f t="shared" si="8"/>
-        <v>1497</v>
-      </c>
-    </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D25" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="8">
+      <c r="F32" s="8">
         <f>F6</f>
         <v>151.08333333333334</v>
       </c>
-      <c r="G25" s="8">
-        <f t="shared" ref="G25:L25" si="9">G6</f>
+      <c r="G32" s="8">
+        <f t="shared" ref="G32:L32" si="14">G6</f>
         <v>323.75</v>
       </c>
-      <c r="H25" s="8">
-        <f t="shared" si="9"/>
+      <c r="H32" s="8">
+        <f t="shared" si="14"/>
         <v>518</v>
       </c>
-      <c r="I25" s="8">
-        <f t="shared" si="9"/>
+      <c r="I32" s="8">
+        <f t="shared" si="14"/>
         <v>777</v>
       </c>
-      <c r="J25" s="8">
-        <f t="shared" si="9"/>
+      <c r="J32" s="8">
+        <f t="shared" si="14"/>
         <v>1122.3333333333333</v>
       </c>
-      <c r="K25" s="8">
-        <f t="shared" si="9"/>
+      <c r="K32" s="8">
+        <f t="shared" si="14"/>
         <v>1124</v>
       </c>
-      <c r="L25" s="8">
-        <f t="shared" si="9"/>
+      <c r="L32" s="8">
+        <f t="shared" si="14"/>
         <v>1686</v>
       </c>
     </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D26" t="s">
+    <row r="33" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>127</v>
+      </c>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36">
+        <v>0.05</v>
+      </c>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36">
+        <v>0.02</v>
+      </c>
+      <c r="L33" s="36"/>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
         <v>128</v>
       </c>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36">
-        <v>0.05</v>
-      </c>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36">
-        <v>0.02</v>
-      </c>
-      <c r="L26" s="36"/>
-    </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D27" t="s">
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36">
+        <v>0.17</v>
+      </c>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="36">
+        <v>0.16</v>
+      </c>
+      <c r="L34" s="36"/>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D35" t="s">
         <v>129</v>
       </c>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36">
-        <v>0.17</v>
-      </c>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36">
-        <v>0.16</v>
-      </c>
-      <c r="L27" s="36"/>
-    </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D28" t="s">
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I35" s="36"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="L35" s="36"/>
+    </row>
+    <row r="37" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D37" t="s">
         <v>130</v>
       </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36">
-        <v>0.3</v>
-      </c>
-      <c r="L28" s="36"/>
-    </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D30" t="s">
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37">
+        <v>1.9</v>
+      </c>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37">
+        <v>1.3</v>
+      </c>
+      <c r="L37" s="37"/>
+    </row>
+    <row r="38" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
         <v>131</v>
       </c>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37">
-        <v>1.9</v>
-      </c>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37">
-        <v>1.3</v>
-      </c>
-      <c r="L30" s="37"/>
-    </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D31" t="s">
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37">
+        <v>5.2</v>
+      </c>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37">
+        <v>6.3</v>
+      </c>
+      <c r="L38" s="37"/>
+    </row>
+    <row r="39" spans="4:12" x14ac:dyDescent="0.35">
+      <c r="D39" t="s">
         <v>132</v>
       </c>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37">
-        <v>5.2</v>
-      </c>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="37">
-        <v>6.3</v>
-      </c>
-      <c r="L31" s="37"/>
-    </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.35">
-      <c r="D32" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37">
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37">
         <v>34.5</v>
       </c>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37">
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37">
         <v>39.9</v>
       </c>
-      <c r="L32" s="37"/>
+      <c r="L39" s="37"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{104B7EC0-3364-4746-885F-9A6B6C0020CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972FC2BC-0260-479C-B829-BE720EA95DB5}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="44">
+        <v>0.875</v>
+      </c>
+      <c r="C6" s="45">
+        <v>0.16119654977038472</v>
+      </c>
+      <c r="D6" s="46">
+        <v>1200.6405999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="44">
+        <v>1</v>
+      </c>
+      <c r="C7" s="48">
+        <v>0.21481405812248527</v>
+      </c>
+      <c r="D7" s="49">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="44">
+        <v>1</v>
+      </c>
+      <c r="C8" s="48">
+        <v>0.18617397382330492</v>
+      </c>
+      <c r="D8" s="49">
+        <v>1386.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="44">
+        <v>1</v>
+      </c>
+      <c r="C9" s="48">
+        <v>8.8449688431933307E-2</v>
+      </c>
+      <c r="D9" s="49">
+        <v>658.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="44">
+        <v>1</v>
+      </c>
+      <c r="C10" s="45">
+        <v>7.4064726837246908E-2</v>
+      </c>
+      <c r="D10" s="46">
+        <v>551.65646036082637</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="44">
+        <v>1</v>
+      </c>
+      <c r="C11" s="45">
+        <v>3.3957408700606762E-2</v>
+      </c>
+      <c r="D11" s="46">
+        <v>252.9250385</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="44">
+        <v>1</v>
+      </c>
+      <c r="C12" s="45">
+        <v>1.100922047877737E-2</v>
+      </c>
+      <c r="D12" s="46">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="44">
+        <v>1</v>
+      </c>
+      <c r="C13" s="50">
+        <v>0.11465700352287651</v>
+      </c>
+      <c r="D13" s="49">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="44">
+        <v>1</v>
+      </c>
+      <c r="C14" s="50">
+        <v>0.11567737031238422</v>
+      </c>
+      <c r="D14" s="49">
+        <v>861.60000010000022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="53">
+        <f t="shared" ref="C15:D15" si="0">SUM(C6:C14)</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="54">
+        <f t="shared" si="0"/>
+        <v>7448.3020989608267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix H2 tank and add assembly operation
</commit_message>
<xml_diff>
--- a/dev/Assumptions and data.xlsx
+++ b/dev/Assumptions and data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sacchi_r\Documents\GitHub\carculator_truck\dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/carculator_truck/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B81B77-F3F3-AB46-8EE7-8EE614EDD2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25830" windowHeight="12540" activeTab="9"/>
+    <workbookView xWindow="4400" yWindow="6400" windowWidth="25840" windowHeight="12540" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICEV engines" sheetId="4" r:id="rId1"/>
@@ -26,10 +27,20 @@
     <sheet name="H2 tank mass" sheetId="14" r:id="rId12"/>
     <sheet name="weight composition of MAN TGX" sheetId="8" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -991,7 +1002,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -1438,8 +1449,8 @@
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Per cent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1457,7 +1468,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1519,7 +1530,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1604,7 +1615,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-CH"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1825,7 +1836,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1863,7 +1874,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1471918991"/>
@@ -1942,7 +1953,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1980,7 +1991,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1478449695"/>
@@ -2021,7 +2032,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2035,7 +2046,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2116,7 +2127,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-CH"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2224,7 +2235,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1471918991"/>
@@ -2286,7 +2297,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1478449695"/>
@@ -2327,7 +2338,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2341,7 +2352,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2403,7 +2414,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4941,7 +4952,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="727404008"/>
@@ -5000,7 +5011,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="727401384"/>
@@ -5046,7 +5057,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5076,7 +5087,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5090,7 +5101,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5152,7 +5163,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5650,7 +5661,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="719097584"/>
@@ -5709,7 +5720,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="719096928"/>
@@ -5751,7 +5762,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5781,7 +5792,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5795,7 +5806,7 @@
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5832,7 +5843,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5858,7 +5868,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5910,7 +5920,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5936,7 +5945,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-CH"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6038,7 +6047,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -6064,7 +6072,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-CH"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6178,7 +6186,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="741568848"/>
@@ -6240,7 +6248,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="792583024"/>
@@ -6257,7 +6265,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6283,13 +6290,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -6297,6 +6303,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -6320,7 +6327,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6334,7 +6341,7 @@
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6371,7 +6378,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6457,7 +6464,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-CH"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -6642,7 +6649,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6680,7 +6687,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="720453928"/>
@@ -6764,7 +6771,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6802,7 +6809,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="720448352"/>
@@ -6843,7 +6850,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6857,7 +6864,7 @@
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6939,7 +6946,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-CH"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -7154,7 +7161,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7192,7 +7199,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="720453928"/>
@@ -7276,7 +7283,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7314,7 +7321,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="720448352"/>
@@ -7355,7 +7362,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7369,7 +7376,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7431,7 +7438,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7516,7 +7523,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-CH"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -7653,7 +7660,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7691,7 +7698,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1471918991"/>
@@ -7770,7 +7777,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7808,7 +7815,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1478449695"/>
@@ -7849,7 +7856,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7863,7 +7870,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8512,7 +8519,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8550,7 +8557,7 @@
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1081512687"/>
@@ -8629,7 +8636,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8667,7 +8674,7 @@
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1132492911"/>
@@ -8709,13 +8716,12 @@
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -8723,6 +8729,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -8749,7 +8756,7 @@
           <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8763,7 +8770,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8800,7 +8807,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8893,7 +8900,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-CH"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -9019,7 +9026,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="502397080"/>
@@ -9081,7 +9088,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="502399376"/>
@@ -9122,7 +9129,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9136,7 +9143,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9178,7 +9185,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9204,7 +9210,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9399,7 +9405,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9425,7 +9430,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9463,7 +9468,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="497924016"/>
@@ -9517,7 +9522,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9543,7 +9547,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9581,7 +9585,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="721442448"/>
@@ -9622,7 +9626,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9636,7 +9640,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9678,7 +9682,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9704,7 +9707,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9875,7 +9878,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9901,7 +9903,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9939,7 +9941,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="497924016"/>
@@ -9993,7 +9995,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10019,7 +10020,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10057,7 +10058,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="721442448"/>
@@ -10098,7 +10099,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10112,7 +10113,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10154,7 +10155,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10180,7 +10180,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -10351,7 +10351,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10377,7 +10376,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10415,7 +10414,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="497924016"/>
@@ -10469,7 +10468,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10495,7 +10493,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10533,7 +10531,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="721442448"/>
@@ -10574,7 +10572,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10588,7 +10586,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10630,7 +10628,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10656,7 +10653,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -10804,7 +10801,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10830,7 +10826,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10868,7 +10864,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="497924016"/>
@@ -10922,7 +10918,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10948,7 +10943,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10986,7 +10981,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="721442448"/>
@@ -11027,7 +11022,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11041,7 +11036,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -11103,7 +11098,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11177,7 +11172,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-CH"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -11326,7 +11321,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11364,7 +11359,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1471918991"/>
@@ -11443,7 +11438,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-CH"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11481,7 +11476,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1478449695"/>
@@ -11522,7 +11517,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -19893,7 +19888,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0908A0C9-570E-4D1F-B76C-96E341C39ECA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19931,7 +19926,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8264ED7-6092-4836-88DA-CA3FF60CC6C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -19964,14 +19959,20 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -20011,7 +20012,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42BDBFEA-B62A-40BE-9BE4-56260E494C43}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20049,7 +20050,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -20087,7 +20094,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023A76B8-635F-4C21-A2E4-6BC7A008B515}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20125,7 +20132,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DE0CF5F-3D00-4073-8083-195BDF7167FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20163,7 +20170,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE34F376-A476-4610-BDCB-350825D1CFB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20201,7 +20208,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023A76B8-635F-4C21-A2E4-6BC7A008B515}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20244,7 +20251,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD0C19C1-03B6-4BA7-BFA2-BCDC52132B74}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20287,7 +20294,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{653354FE-C245-430C-8E82-2CBB529D8844}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20327,7 +20334,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -20357,7 +20370,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -20395,7 +20414,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98A7E4CB-2BD3-49C0-A8F4-0A3628A02352}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -20433,7 +20452,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -20747,14 +20772,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
@@ -21014,20 +21039,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="161" customWidth="1"/>
-    <col min="12" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="161" customWidth="1"/>
+    <col min="12" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -21069,7 +21094,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="38.25">
+    <row r="5" spans="1:13" ht="30">
       <c r="E5" t="s">
         <v>90</v>
       </c>
@@ -21671,35 +21696,35 @@
         <v>91</v>
       </c>
       <c r="F22" s="8">
-        <f>F18</f>
+        <f t="shared" ref="F22:M22" si="10">F18</f>
         <v>583.33333333333337</v>
       </c>
       <c r="G22" s="8">
-        <f>G18</f>
+        <f t="shared" si="10"/>
         <v>1250</v>
       </c>
       <c r="H22" s="8">
-        <f>H18</f>
+        <f t="shared" si="10"/>
         <v>2000</v>
       </c>
       <c r="I22" s="8">
-        <f>I18</f>
+        <f t="shared" si="10"/>
         <v>3000</v>
       </c>
       <c r="J22" s="8">
-        <f>J18</f>
+        <f t="shared" si="10"/>
         <v>4333.333333333333</v>
       </c>
       <c r="K22" s="8">
-        <f>K18</f>
+        <f t="shared" si="10"/>
         <v>1680</v>
       </c>
       <c r="L22" s="8">
-        <f>L18</f>
+        <f t="shared" si="10"/>
         <v>2100</v>
       </c>
       <c r="M22" s="8">
-        <f>M18</f>
+        <f t="shared" si="10"/>
         <v>3150</v>
       </c>
     </row>
@@ -21708,23 +21733,23 @@
         <v>93</v>
       </c>
       <c r="F23" s="26">
-        <f t="shared" ref="F23:L23" si="10">F22/F20</f>
+        <f t="shared" ref="F23:L23" si="11">F22/F20</f>
         <v>0.31501023783272958</v>
       </c>
       <c r="G23" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.31501023783272958</v>
       </c>
       <c r="H23" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.31501023783272958</v>
       </c>
       <c r="I23" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.31501023783272958</v>
       </c>
       <c r="J23" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.33053648614289349</v>
       </c>
       <c r="K23" s="26">
@@ -21732,7 +21757,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="L23" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="M23" s="26">
@@ -21786,31 +21811,31 @@
         <v>82.541666666666671</v>
       </c>
       <c r="G26" s="8">
-        <f t="shared" ref="G26:M26" si="11">SUM(G11)</f>
+        <f t="shared" ref="G26:M26" si="12">SUM(G11)</f>
         <v>176.875</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>283</v>
       </c>
       <c r="I26" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>424.5</v>
       </c>
       <c r="J26" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>613.16666666666663</v>
       </c>
       <c r="K26" s="8">
-        <f t="shared" ref="K26" si="12">SUM(K11)</f>
+        <f t="shared" ref="K26" si="13">SUM(K11)</f>
         <v>446.4</v>
       </c>
       <c r="L26" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>558</v>
       </c>
       <c r="M26" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>837</v>
       </c>
     </row>
@@ -21823,31 +21848,31 @@
         <v>151.08333333333334</v>
       </c>
       <c r="G27" s="8">
-        <f t="shared" ref="G27:M27" si="13">G7</f>
+        <f t="shared" ref="G27:M27" si="14">G7</f>
         <v>323.75</v>
       </c>
       <c r="H27" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>518</v>
       </c>
       <c r="I27" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>777</v>
       </c>
       <c r="J27" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1122.3333333333333</v>
       </c>
       <c r="K27" s="8">
-        <f t="shared" ref="K27" si="14">K7</f>
+        <f t="shared" ref="K27" si="15">K7</f>
         <v>899.2</v>
       </c>
       <c r="L27" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1124</v>
       </c>
       <c r="M27" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1686</v>
       </c>
     </row>
@@ -21955,7 +21980,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -21964,19 +21989,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -22295,7 +22320,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -22303,21 +22328,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -22656,16 +22681,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -22673,7 +22698,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="16">
       <c r="A5" s="27" t="s">
         <v>66</v>
       </c>
@@ -22799,7 +22824,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1">
+    <row r="14" spans="1:4" ht="16" thickBot="1">
       <c r="A14" s="32" t="s">
         <v>35</v>
       </c>
@@ -22813,7 +22838,7 @@
         <v>861.60000010000022</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1">
+    <row r="15" spans="1:4" ht="16" thickBot="1">
       <c r="A15" s="36" t="s">
         <v>76</v>
       </c>
@@ -22833,14 +22858,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D7:AE25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="7" spans="5:24">
       <c r="F7" t="s">
@@ -23258,27 +23283,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="42" t="s">
         <v>99</v>
       </c>
@@ -23310,7 +23335,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1">
+    <row r="2" spans="1:10" ht="16" thickTop="1">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -23958,19 +23983,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1"/>
-    <hyperlink ref="J2" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6"/>
-    <hyperlink ref="J8" r:id="rId7"/>
-    <hyperlink ref="J9" r:id="rId8"/>
-    <hyperlink ref="J10" r:id="rId9"/>
-    <hyperlink ref="J11" r:id="rId10"/>
-    <hyperlink ref="J12" r:id="rId11"/>
-    <hyperlink ref="J13" r:id="rId12"/>
-    <hyperlink ref="J14" r:id="rId13"/>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="J11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="J12" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="J13" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="J14" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
@@ -23978,22 +24003,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AV37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" style="161" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" style="161" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48">
@@ -25830,8 +25855,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R4" r:id="rId1"/>
-    <hyperlink ref="R5" r:id="rId2"/>
+    <hyperlink ref="R4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="R5" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>
@@ -25839,29 +25864,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1">
+    <row r="1" spans="1:14" ht="16" thickBot="1">
       <c r="A1" s="42" t="s">
         <v>99</v>
       </c>
@@ -25905,7 +25930,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickTop="1">
+    <row r="2" spans="1:14" ht="16" thickTop="1">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -26333,9 +26358,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1"/>
-    <hyperlink ref="N9" r:id="rId2"/>
-    <hyperlink ref="N10:N12" r:id="rId3" display="https://www.mdpi.com/2032-6653/11/1/12/pdf"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="N9" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="N10:N12" r:id="rId3" display="https://www.mdpi.com/2032-6653/11/1/12/pdf" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -26344,27 +26369,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="42" t="s">
         <v>99</v>
       </c>
@@ -26402,7 +26427,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickTop="1">
+    <row r="2" spans="1:12" ht="16" thickTop="1">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -26657,29 +26682,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
-    <hyperlink ref="L5" r:id="rId4"/>
-    <hyperlink ref="L6" r:id="rId5"/>
-    <hyperlink ref="L7" r:id="rId6"/>
-    <hyperlink ref="L8" r:id="rId7"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="L6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="L7" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="L8" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -26758,14 +26783,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
@@ -26814,17 +26839,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="58.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">

</xml_diff>